<commit_message>
Added failsafe for the excel file
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -30034,28 +30034,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>65449.16666666675</v>
+        <v>65514.58333333342</v>
       </c>
       <c r="C3" t="n">
-        <v>7160.416666666693</v>
+        <v>7225.833333333358</v>
       </c>
       <c r="D3" t="n">
         <v>58288.75000000006</v>
       </c>
       <c r="E3" t="n">
-        <v>7160.416666666693</v>
+        <v>7225.833333333358</v>
       </c>
       <c r="F3" t="n">
         <v>58288.75000000006</v>
       </c>
       <c r="G3" t="n">
-        <v>7160.416666666693</v>
+        <v>7225.833333333358</v>
       </c>
       <c r="H3" t="n">
         <v>58288.75000000006</v>
       </c>
       <c r="I3" t="n">
-        <v>7160.416666666693</v>
+        <v>7225.833333333358</v>
       </c>
       <c r="J3" t="n">
         <v>58288.75000000006</v>
@@ -30136,28 +30136,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16832</v>
+        <v>16845</v>
       </c>
       <c r="C6" t="n">
-        <v>2504</v>
+        <v>2517</v>
       </c>
       <c r="D6" t="n">
         <v>14328</v>
       </c>
       <c r="E6" t="n">
-        <v>2504</v>
+        <v>2517</v>
       </c>
       <c r="F6" t="n">
         <v>14328</v>
       </c>
       <c r="G6" t="n">
-        <v>2504</v>
+        <v>2517</v>
       </c>
       <c r="H6" t="n">
         <v>14328</v>
       </c>
       <c r="I6" t="n">
-        <v>2504</v>
+        <v>2517</v>
       </c>
       <c r="J6" t="n">
         <v>14328</v>
@@ -30238,28 +30238,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C9" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D9" t="n">
         <v>562</v>
       </c>
       <c r="E9" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F9" t="n">
         <v>562</v>
       </c>
       <c r="G9" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H9" t="n">
         <v>562</v>
       </c>
       <c r="I9" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J9" t="n">
         <v>562</v>
@@ -30306,28 +30306,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6255</v>
+        <v>6263</v>
       </c>
       <c r="C11" t="n">
-        <v>946</v>
+        <v>954</v>
       </c>
       <c r="D11" t="n">
         <v>5309</v>
       </c>
       <c r="E11" t="n">
-        <v>946</v>
+        <v>954</v>
       </c>
       <c r="F11" t="n">
         <v>5309</v>
       </c>
       <c r="G11" t="n">
-        <v>946</v>
+        <v>954</v>
       </c>
       <c r="H11" t="n">
         <v>5309</v>
       </c>
       <c r="I11" t="n">
-        <v>946</v>
+        <v>954</v>
       </c>
       <c r="J11" t="n">
         <v>5309</v>
@@ -30408,28 +30408,28 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C14" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D14" t="n">
         <v>425</v>
       </c>
       <c r="E14" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F14" t="n">
         <v>425</v>
       </c>
       <c r="G14" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H14" t="n">
         <v>425</v>
       </c>
       <c r="I14" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J14" t="n">
         <v>425</v>
@@ -30442,28 +30442,28 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C15" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D15" t="n">
         <v>592</v>
       </c>
       <c r="E15" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F15" t="n">
         <v>592</v>
       </c>
       <c r="G15" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H15" t="n">
         <v>592</v>
       </c>
       <c r="I15" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J15" t="n">
         <v>592</v>
@@ -30646,28 +30646,28 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n">
         <v>38</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F21" t="n">
         <v>38</v>
       </c>
       <c r="G21" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H21" t="n">
         <v>38</v>
       </c>
       <c r="I21" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J21" t="n">
         <v>38</v>
@@ -30680,28 +30680,28 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>68412</v>
+        <v>68485</v>
       </c>
       <c r="C22" t="n">
-        <v>9337</v>
+        <v>9410</v>
       </c>
       <c r="D22" t="n">
         <v>59075</v>
       </c>
       <c r="E22" t="n">
-        <v>9337</v>
+        <v>9410</v>
       </c>
       <c r="F22" t="n">
         <v>59075</v>
       </c>
       <c r="G22" t="n">
-        <v>9337</v>
+        <v>9410</v>
       </c>
       <c r="H22" t="n">
         <v>59075</v>
       </c>
       <c r="I22" t="n">
-        <v>9337</v>
+        <v>9410</v>
       </c>
       <c r="J22" t="n">
         <v>59075</v>

</xml_diff>